<commit_message>
corrected inf value in GeneratorsVariables
</commit_message>
<xml_diff>
--- a/DownloadDataForDK/ModelData/Final_Dataset/GeneratorsVariables.xlsx
+++ b/DownloadDataForDK/ModelData/Final_Dataset/GeneratorsVariables.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="121">
   <si>
     <t>FuelMix/id</t>
   </si>
@@ -272,9 +272,6 @@
   </si>
   <si>
     <t>Waste</t>
-  </si>
-  <si>
-    <t>inf</t>
   </si>
   <si>
     <t>DK2_SmallDecentral_BP_Oil</t>
@@ -924,7 +921,7 @@
         <v>598.211</v>
       </c>
       <c r="F5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G5">
         <v>7.355</v>
@@ -1065,7 +1062,7 @@
         <v>18871.99865918949</v>
       </c>
       <c r="L8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M8">
         <v>-10</v>
@@ -1088,25 +1085,25 @@
         <v>13.281</v>
       </c>
       <c r="F9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G9">
         <v>2</v>
       </c>
       <c r="H9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M9">
         <v>-0.2808402594568861</v>
@@ -1129,7 +1126,7 @@
         <v>340.864</v>
       </c>
       <c r="F10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G10">
         <v>100.826</v>
@@ -1147,7 +1144,7 @@
         <v>41780.64064438807</v>
       </c>
       <c r="L10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M10">
         <v>-0.2471153414447986</v>
@@ -1170,7 +1167,7 @@
         <v>0.195</v>
       </c>
       <c r="F11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G11">
         <v>44.546</v>
@@ -1188,7 +1185,7 @@
         <v>146939.6312029963</v>
       </c>
       <c r="L11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M11">
         <v>-1</v>
@@ -1211,7 +1208,7 @@
         <v>34.192</v>
       </c>
       <c r="F12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G12">
         <v>560.42</v>
@@ -1252,7 +1249,7 @@
         <v>40.033</v>
       </c>
       <c r="F13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G13">
         <v>248.8</v>
@@ -1293,7 +1290,7 @@
         <v>9.721</v>
       </c>
       <c r="F14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G14">
         <v>4.1</v>
@@ -1340,10 +1337,10 @@
         <v>0.5</v>
       </c>
       <c r="H15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L15" t="s">
         <v>34</v>
@@ -1375,13 +1372,13 @@
         <v>1.61</v>
       </c>
       <c r="H16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I16">
         <v>2.300976353351277</v>
       </c>
       <c r="J16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K16">
         <v>2101.34826790071</v>
@@ -1416,19 +1413,19 @@
         <v>545.326</v>
       </c>
       <c r="H17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I17">
         <v>2.300976353351277</v>
       </c>
       <c r="J17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K17">
         <v>2101.34826790071</v>
       </c>
       <c r="L17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M17">
         <v>-10</v>
@@ -1451,19 +1448,19 @@
         <v>5.35</v>
       </c>
       <c r="H18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I18">
         <v>0.4903145958434989</v>
       </c>
       <c r="J18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K18">
         <v>1110.212334874208</v>
       </c>
       <c r="L18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M18">
         <v>-0.3113682161510096</v>
@@ -1486,19 +1483,19 @@
         <v>896.681</v>
       </c>
       <c r="H19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I19">
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
       <c r="L19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M19">
         <v>-0.1848692749860931</v>
@@ -1521,19 +1518,19 @@
         <v>355.433</v>
       </c>
       <c r="H20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I20">
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K20">
         <v>63.66022069579798</v>
       </c>
       <c r="L20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M20">
         <v>-1</v>
@@ -1585,7 +1582,7 @@
         <v>1.150943396226415</v>
       </c>
       <c r="F22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G22">
         <v>7.8</v>
@@ -1620,7 +1617,7 @@
         <v>20</v>
       </c>
       <c r="F23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G23">
         <v>8.300000000000001</v>
@@ -1655,7 +1652,7 @@
         <v>0.9385964912280701</v>
       </c>
       <c r="F24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G24">
         <v>72.949</v>
@@ -1690,7 +1687,7 @@
         <v>8.126213592233009</v>
       </c>
       <c r="F25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G25">
         <v>10.786</v>
@@ -1725,7 +1722,7 @@
         <v>1.857142857142857</v>
       </c>
       <c r="F26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G26">
         <v>192.3</v>
@@ -1743,7 +1740,7 @@
         <v>0</v>
       </c>
       <c r="L26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M26">
         <v>-10</v>
@@ -1760,7 +1757,7 @@
         <v>2.567375886524823</v>
       </c>
       <c r="F27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G27">
         <v>14.5</v>
@@ -1778,7 +1775,7 @@
         <v>1908.724676676478</v>
       </c>
       <c r="L27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M27">
         <v>-0.2929720248650695</v>
@@ -1795,7 +1792,7 @@
         <v>0.5757575757575757</v>
       </c>
       <c r="F28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G28">
         <v>139</v>
@@ -1813,7 +1810,7 @@
         <v>18871.99865918949</v>
       </c>
       <c r="L28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M28">
         <v>-0.2080392391434382</v>
@@ -1854,7 +1851,7 @@
         <v>41780.64064438807</v>
       </c>
       <c r="L29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M29">
         <v>-1</v>
@@ -2006,10 +2003,10 @@
         <v>1308.327</v>
       </c>
       <c r="H33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L33" t="s">
         <v>59</v>
@@ -2041,13 +2038,13 @@
         <v>1.264</v>
       </c>
       <c r="H34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I34">
         <v>2.663131119234357</v>
       </c>
       <c r="J34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K34">
         <v>14919.57270209504</v>
@@ -2082,19 +2079,19 @@
         <v>456.711</v>
       </c>
       <c r="H35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I35">
         <v>2.300976353351277</v>
       </c>
       <c r="J35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K35">
         <v>2101.34826790071</v>
       </c>
       <c r="L35" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M35">
         <v>-0.2901974951830443</v>
@@ -2123,19 +2120,19 @@
         <v>1.102</v>
       </c>
       <c r="H36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I36">
         <v>2.300976353351277</v>
       </c>
       <c r="J36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K36">
         <v>2101.34826790071</v>
       </c>
       <c r="L36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M36">
         <v>-0.1658761528326746</v>
@@ -2164,19 +2161,19 @@
         <v>6.284</v>
       </c>
       <c r="H37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I37">
         <v>0.4903145958434989</v>
       </c>
       <c r="J37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K37">
         <v>1110.212334874208</v>
       </c>
       <c r="L37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M37">
         <v>-1</v>
@@ -2199,19 +2196,19 @@
         <v>13.327</v>
       </c>
       <c r="F38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G38">
         <v>1</v>
       </c>
       <c r="H38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I38">
         <v>0</v>
       </c>
       <c r="J38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K38">
         <v>0</v>
@@ -2240,19 +2237,19 @@
         <v>21.986</v>
       </c>
       <c r="F39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G39">
         <v>258.837</v>
       </c>
       <c r="H39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I39">
         <v>0</v>
       </c>
       <c r="J39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K39">
         <v>63.66022069579798</v>
@@ -2398,7 +2395,7 @@
         <v>0</v>
       </c>
       <c r="L43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M43">
         <v>0.45</v>
@@ -2433,7 +2430,7 @@
         <v>41780.64064438807</v>
       </c>
       <c r="L44" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M44">
         <v>-0.309554234769688</v>
@@ -2450,7 +2447,7 @@
         <v>1.12</v>
       </c>
       <c r="F45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G45">
         <v>41.52</v>
@@ -2468,7 +2465,7 @@
         <v>146939.6312029963</v>
       </c>
       <c r="L45" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M45">
         <v>-1</v>
@@ -2485,7 +2482,7 @@
         <v>2.546153846153846</v>
       </c>
       <c r="F46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G46">
         <v>15.18</v>
@@ -2514,7 +2511,7 @@
         <v>1.129787234042553</v>
       </c>
       <c r="F47" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G47">
         <v>205.2</v>
@@ -2543,7 +2540,7 @@
         <v>5.588235294117647</v>
       </c>
       <c r="F48" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G48">
         <v>0.9</v>
@@ -2572,16 +2569,16 @@
         <v>1.178571428571429</v>
       </c>
       <c r="F49" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G49">
         <v>2.1</v>
       </c>
       <c r="H49" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J49" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -2601,13 +2598,13 @@
         <v>1.33</v>
       </c>
       <c r="H50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I50">
         <v>2.300976353351277</v>
       </c>
       <c r="J50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K50">
         <v>2101.34826790071</v>
@@ -2630,13 +2627,13 @@
         <v>169.194</v>
       </c>
       <c r="H51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I51">
         <v>2.300976353351277</v>
       </c>
       <c r="J51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K51">
         <v>2101.34826790071</v>
@@ -2659,13 +2656,13 @@
         <v>609.367</v>
       </c>
       <c r="H52" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I52">
         <v>0.4903145958434989</v>
       </c>
       <c r="J52" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K52">
         <v>1110.212334874208</v>
@@ -2688,13 +2685,13 @@
         <v>57.83</v>
       </c>
       <c r="H53" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I53">
         <v>0</v>
       </c>
       <c r="J53" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K53">
         <v>0</v>
@@ -2717,13 +2714,13 @@
         <v>8.346</v>
       </c>
       <c r="H54" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I54">
         <v>0</v>
       </c>
       <c r="J54" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K54">
         <v>63.66022069579798</v>
@@ -2740,7 +2737,7 @@
         <v>2.875</v>
       </c>
       <c r="F55" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G55">
         <v>25</v>
@@ -2757,7 +2754,7 @@
         <v>1.142857142857143</v>
       </c>
       <c r="F56" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G56">
         <v>0.9</v>
@@ -2770,11 +2767,11 @@
       <c r="B57" t="s">
         <v>84</v>
       </c>
-      <c r="C57" t="s">
-        <v>86</v>
+      <c r="C57">
+        <v>20</v>
       </c>
       <c r="F57" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G57">
         <v>40</v>
@@ -2791,7 +2788,7 @@
         <v>1.272727272727273</v>
       </c>
       <c r="F58" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G58">
         <v>2</v>
@@ -2808,7 +2805,7 @@
         <v>6.273972602739726</v>
       </c>
       <c r="F59" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G59">
         <v>2.88</v>
@@ -2927,7 +2924,7 @@
         <v>2.518518518518519</v>
       </c>
       <c r="F66" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G66">
         <v>67.3</v>
@@ -2956,7 +2953,7 @@
         <v>1.125</v>
       </c>
       <c r="F67" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G67">
         <v>87.3</v>
@@ -2985,7 +2982,7 @@
         <v>1.15</v>
       </c>
       <c r="F68" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G68">
         <v>19.3</v>
@@ -3011,7 +3008,7 @@
         <v>101.657</v>
       </c>
       <c r="F69" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G69">
         <v>8.359</v>
@@ -3037,13 +3034,13 @@
     </row>
     <row r="70" spans="1:13">
       <c r="D70" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E70">
         <v>0.008999999999999999</v>
       </c>
       <c r="F70" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G70">
         <v>482.13</v>
@@ -3069,7 +3066,7 @@
     </row>
     <row r="71" spans="1:13">
       <c r="F71" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G71">
         <v>76.62</v>
@@ -3087,7 +3084,7 @@
         <v>0</v>
       </c>
       <c r="L71" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M71">
         <v>-0.29412</v>
@@ -3095,7 +3092,7 @@
     </row>
     <row r="72" spans="1:13">
       <c r="F72" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G72">
         <v>780.0309999999999</v>
@@ -3113,7 +3110,7 @@
         <v>40675.09797233142</v>
       </c>
       <c r="L72" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M72">
         <v>-0.1855555555555556</v>
@@ -3139,7 +3136,7 @@
         <v>213076.714365132</v>
       </c>
       <c r="L73" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M73">
         <v>-1</v>
@@ -3147,7 +3144,7 @@
     </row>
     <row r="74" spans="1:13">
       <c r="F74" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G74">
         <v>179.046</v>
@@ -3265,13 +3262,13 @@
     </row>
     <row r="82" spans="8:11">
       <c r="H82" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I82">
         <v>2.300976353351277</v>
       </c>
       <c r="J82" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K82">
         <v>2101.34826790071</v>
@@ -3279,13 +3276,13 @@
     </row>
     <row r="83" spans="8:11">
       <c r="H83" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I83">
         <v>2.300976353351277</v>
       </c>
       <c r="J83" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K83">
         <v>2101.34826790071</v>
@@ -3293,13 +3290,13 @@
     </row>
     <row r="84" spans="8:11">
       <c r="H84" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I84">
         <v>0.4903145958434989</v>
       </c>
       <c r="J84" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K84">
         <v>1110.212334874208</v>
@@ -3307,13 +3304,13 @@
     </row>
     <row r="85" spans="8:11">
       <c r="H85" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I85">
         <v>0</v>
       </c>
       <c r="J85" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K85">
         <v>0</v>
@@ -3321,13 +3318,13 @@
     </row>
     <row r="86" spans="8:11">
       <c r="H86" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I86">
         <v>0</v>
       </c>
       <c r="J86" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K86">
         <v>63.66022069579798</v>
@@ -3461,13 +3458,13 @@
     </row>
     <row r="96" spans="8:11">
       <c r="H96" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I96">
         <v>2.300976353351277</v>
       </c>
       <c r="J96" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K96">
         <v>2101.34826790071</v>
@@ -3475,13 +3472,13 @@
     </row>
     <row r="97" spans="8:11">
       <c r="H97" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I97">
         <v>2.300976353351277</v>
       </c>
       <c r="J97" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K97">
         <v>2101.34826790071</v>
@@ -3489,13 +3486,13 @@
     </row>
     <row r="98" spans="8:11">
       <c r="H98" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I98">
         <v>0.4903145958434989</v>
       </c>
       <c r="J98" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K98">
         <v>1110.212334874208</v>
@@ -3503,13 +3500,13 @@
     </row>
     <row r="99" spans="8:11">
       <c r="H99" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I99">
         <v>0</v>
       </c>
       <c r="J99" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K99">
         <v>0</v>
@@ -3517,13 +3514,13 @@
     </row>
     <row r="100" spans="8:11">
       <c r="H100" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I100">
         <v>0</v>
       </c>
       <c r="J100" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K100">
         <v>63.66022069579798</v>
@@ -3643,13 +3640,13 @@
     </row>
     <row r="109" spans="8:11">
       <c r="H109" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I109">
         <v>11.02137867397912</v>
       </c>
       <c r="J109" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K109">
         <v>146939.6312029963</v>
@@ -3671,13 +3668,13 @@
     </row>
     <row r="111" spans="8:11">
       <c r="H111" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I111">
         <v>2.300976353351277</v>
       </c>
       <c r="J111" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K111">
         <v>2101.34826790071</v>
@@ -3685,13 +3682,13 @@
     </row>
     <row r="112" spans="8:11">
       <c r="H112" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I112">
         <v>0.4903145958434989</v>
       </c>
       <c r="J112" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K112">
         <v>1110.212334874208</v>
@@ -3699,13 +3696,13 @@
     </row>
     <row r="113" spans="8:11">
       <c r="H113" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I113">
         <v>0</v>
       </c>
       <c r="J113" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K113">
         <v>0</v>
@@ -3713,13 +3710,13 @@
     </row>
     <row r="114" spans="8:11">
       <c r="H114" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I114">
         <v>0</v>
       </c>
       <c r="J114" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K114">
         <v>63.66022069579798</v>

</xml_diff>

<commit_message>
finalising constructing aggregated data
</commit_message>
<xml_diff>
--- a/DownloadDataForDK/ModelData/Final_Dataset/GeneratorsVariables.xlsx
+++ b/DownloadDataForDK/ModelData/Final_Dataset/GeneratorsVariables.xlsx
@@ -471,12 +471,12 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>OtherMC/id</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>OtherMC</t>
+          <t>OtherMC/OtherMC</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">

</xml_diff>